<commit_message>
Asdf data new added
</commit_message>
<xml_diff>
--- a/data/2024_2.xlsx
+++ b/data/2024_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28007"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A_오션ICT_학생제출\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63A27E11-D8C5-4268-BA11-5193763B5C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8BFA872-0F22-43D3-9D7F-50149353A68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{65DE6A28-D80C-427F-AA88-4E0774EDEF8A}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="391">
   <si>
     <t>제7회 BSS Ocean ICT Festival 참가자 명단(팀별)_96팀</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -164,7 +164,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>링크 주소 이상내용_0813</t>
+    <t>링크 주소 이상내용_0813 / 0814</t>
   </si>
   <si>
     <t>누락된 내용_0805</t>
@@ -408,7 +408,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>팀즈 파일 없음</t>
+    <t>https://www.youtube.com/watch?v=xinzoji8sbU</t>
   </si>
   <si>
     <t>별미</t>
@@ -427,6 +427,9 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>https://youtu.be/cuQ1bILptjw?si=s93SbFUMLrUdB6PU</t>
+  </si>
+  <si>
     <t>오진우뭐먹어나도줘</t>
   </si>
   <si>
@@ -551,11 +554,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>https://m.site.naver.com/1qLyY</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>제목 양식</t>
+    <t>https://www.youtube.com/watch?app=desktop&amp;v=aL62t6nsk4Y</t>
   </si>
   <si>
     <t>해병</t>
@@ -710,7 +709,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>https://youtu.be/3lUMRPj2vdE?si=X2-ZXOJjziPcpLqn</t>
+    <t>https://www.youtube.com/watch?si=X2-ZXOJjziPcpLqn&amp;v=3lUMRPj2vdE&amp;feature=youtu.be</t>
   </si>
   <si>
     <t>썸네일</t>
@@ -724,11 +723,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>https://youtu.be/BReIj2NSqHw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>잘못된 동영상</t>
+    <t>https://youtu.be/FJNCCRCqKKs?si=vcTIssEXQ7bjR6ar</t>
   </si>
   <si>
     <t>온도와 해류 변화에 따른 성게 서식지 변화 예측</t>
@@ -1338,11 +1333,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>https://youtu.be/YG1i9N3xv5M?si=GOrccz7jmdswt2Xb</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>일부 공개</t>
+    <t>https://youtu.be/-arx11iPcXo?si=ZwjScksFl11Bmqn_</t>
   </si>
   <si>
     <t>해저 광물 자원 채굴의 경제적 잠재력 분석</t>
@@ -1375,9 +1366,6 @@
   </si>
   <si>
     <t>https://m.site.naver.com/1qSEG</t>
-  </si>
-  <si>
-    <t>영상 링크 큐알 안 열림</t>
   </si>
   <si>
     <t>수온와 수심 등의 변화에 따른 최적의 양식장 위치 변화 예측</t>
@@ -1487,7 +1475,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1495,14 +1483,14 @@
       <b/>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1511,14 +1499,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1526,7 +1514,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1535,7 +1523,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1550,7 +1538,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1569,7 +1557,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFF00"/>
-      <name val="맑은 고딕"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1771,7 +1759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1834,9 +1822,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2547,117 +2532,117 @@
   </sheetPr>
   <dimension ref="A1:T105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D41" sqref="D39:D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="7.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="7.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.875" style="1" customWidth="1"/>
-    <col min="7" max="12" width="10.125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="21.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="1" customWidth="1"/>
+    <col min="7" max="12" width="10.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="27" style="1" customWidth="1"/>
-    <col min="15" max="19" width="6.375" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="43.5" style="1" customWidth="1"/>
+    <col min="15" max="19" width="6.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="43.42578125" style="1" customWidth="1"/>
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="32.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:20" ht="29.25">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
     </row>
     <row r="2" spans="1:20" ht="22.5" customHeight="1"/>
     <row r="3" spans="1:20">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="39" t="s">
+      <c r="I3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="39" t="s">
+      <c r="L3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="N3" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="41" t="s">
+      <c r="O3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="39" t="s">
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="38" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="32.25" customHeight="1">
-      <c r="A4" s="40"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
       <c r="O4" s="4" t="s">
         <v>16</v>
       </c>
@@ -2673,9 +2658,9 @@
       <c r="S4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="40"/>
-    </row>
-    <row r="5" spans="1:20" ht="33">
+      <c r="T4" s="39"/>
+    </row>
+    <row r="5" spans="1:20" ht="30.75">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2685,8 +2670,8 @@
       <c r="C5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="23" t="s">
+      <c r="D5" s="26"/>
+      <c r="E5" s="22" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="7">
@@ -2721,7 +2706,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" ht="15.75">
       <c r="A6" s="6">
         <v>13</v>
       </c>
@@ -2731,13 +2716,13 @@
       <c r="C6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="7">
         <v>1</v>
       </c>
       <c r="G6" s="7">
-        <v>6666</v>
+        <v>1208</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="8">
@@ -2765,7 +2750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="33">
+    <row r="7" spans="1:20" ht="27.75">
       <c r="A7" s="6">
         <v>21</v>
       </c>
@@ -2775,8 +2760,8 @@
       <c r="C7" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="25" t="s">
+      <c r="D7" s="26"/>
+      <c r="E7" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="7">
@@ -2813,7 +2798,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="33">
+    <row r="8" spans="1:20" ht="30.75">
       <c r="A8" s="6">
         <v>22</v>
       </c>
@@ -2823,8 +2808,8 @@
       <c r="C8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="25" t="s">
+      <c r="D8" s="26"/>
+      <c r="E8" s="24" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="7">
@@ -2859,7 +2844,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="33">
+    <row r="9" spans="1:20" ht="27.75">
       <c r="A9" s="6">
         <v>88</v>
       </c>
@@ -2869,8 +2854,8 @@
       <c r="C9" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="26"/>
+      <c r="E9" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="10">
@@ -2907,7 +2892,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="33">
+    <row r="10" spans="1:20" ht="27.75">
       <c r="A10" s="6">
         <v>27</v>
       </c>
@@ -2917,8 +2902,8 @@
       <c r="C10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="7">
         <v>1</v>
       </c>
@@ -2951,7 +2936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" ht="15.75">
       <c r="A11" s="6">
         <v>39</v>
       </c>
@@ -2961,8 +2946,8 @@
       <c r="C11" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="24"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="12">
         <v>2</v>
       </c>
@@ -2991,7 +2976,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="33">
+    <row r="12" spans="1:20" ht="30.75">
       <c r="A12" s="6">
         <v>60</v>
       </c>
@@ -3001,8 +2986,8 @@
       <c r="C12" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="24"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="12">
         <v>2</v>
       </c>
@@ -3035,7 +3020,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="33">
+    <row r="13" spans="1:20" ht="27.75">
       <c r="A13" s="6">
         <v>63</v>
       </c>
@@ -3045,8 +3030,8 @@
       <c r="C13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="24"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="12">
         <v>2</v>
       </c>
@@ -3075,7 +3060,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="33">
+    <row r="14" spans="1:20" ht="15.75">
       <c r="A14" s="6">
         <v>68</v>
       </c>
@@ -3085,8 +3070,8 @@
       <c r="C14" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="25" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="24" t="s">
         <v>38</v>
       </c>
       <c r="F14" s="12">
@@ -3119,7 +3104,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="33">
+    <row r="15" spans="1:20" ht="27.75">
       <c r="A15" s="6">
         <v>82</v>
       </c>
@@ -3129,8 +3114,8 @@
       <c r="C15" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="23" t="s">
+      <c r="D15" s="26"/>
+      <c r="E15" s="22" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="10">
@@ -3163,7 +3148,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" ht="15.75">
       <c r="A16" s="6">
         <v>1</v>
       </c>
@@ -3173,8 +3158,8 @@
       <c r="C16" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="25"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="7">
         <v>1</v>
       </c>
@@ -3205,7 +3190,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="33">
+    <row r="17" spans="1:20" ht="27.75">
       <c r="A17" s="6">
         <v>2</v>
       </c>
@@ -3215,8 +3200,8 @@
       <c r="C17" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="25"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="7">
         <v>1</v>
       </c>
@@ -3247,7 +3232,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="49.5">
+    <row r="18" spans="1:20" ht="41.25">
       <c r="A18" s="6">
         <v>3</v>
       </c>
@@ -3257,8 +3242,8 @@
       <c r="C18" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="25"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="7">
         <v>1</v>
       </c>
@@ -3291,18 +3276,18 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="49.5">
+    <row r="19" spans="1:20" ht="41.25">
       <c r="A19" s="6">
         <v>5</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="D19" s="26"/>
+      <c r="E19" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F19" s="7">
@@ -3335,18 +3320,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" ht="27.75">
       <c r="A20" s="6">
         <v>6</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="25" t="s">
+      <c r="C20" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="7">
@@ -3363,7 +3348,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N20" s="9" t="s">
         <v>73</v>
@@ -3378,21 +3363,21 @@
       </c>
       <c r="S20" s="6"/>
       <c r="T20" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="33">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="15.75">
       <c r="A21" s="6">
         <v>7</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="25"/>
+        <v>93</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="7">
         <v>1</v>
       </c>
@@ -3407,7 +3392,7 @@
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N21" s="9" t="s">
         <v>73</v>
@@ -3420,22 +3405,22 @@
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
       <c r="T21" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="33">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="30.75">
       <c r="A22" s="6">
         <v>9</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="25" t="s">
         <v>97</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="24" t="s">
+        <v>98</v>
       </c>
       <c r="F22" s="7">
         <v>1</v>
@@ -3451,7 +3436,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N22" s="9" t="s">
         <v>73</v>
@@ -3464,21 +3449,21 @@
       </c>
       <c r="S22" s="6"/>
       <c r="T22" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="30.75">
       <c r="A23" s="6">
         <v>10</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="25"/>
+        <v>102</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="7">
         <v>1</v>
       </c>
@@ -3493,7 +3478,7 @@
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N23" s="9" t="s">
         <v>73</v>
@@ -3508,21 +3493,21 @@
       </c>
       <c r="S23" s="6"/>
       <c r="T23" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="49.5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="45.75">
       <c r="A24" s="6">
         <v>16</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="25"/>
+        <v>106</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="7">
         <v>1</v>
       </c>
@@ -3537,7 +3522,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N24" s="9" t="s">
         <v>73</v>
@@ -3552,21 +3537,21 @@
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="15.75">
       <c r="A25" s="6">
         <v>17</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="25"/>
+        <v>110</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="7">
         <v>1</v>
       </c>
@@ -3581,7 +3566,7 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N25" s="9" t="s">
         <v>86</v>
@@ -3594,21 +3579,21 @@
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
       <c r="T25" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="49.5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="30.75">
       <c r="A26" s="6">
         <v>18</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="25"/>
+        <v>114</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="24"/>
       <c r="F26" s="7">
         <v>1</v>
       </c>
@@ -3623,7 +3608,7 @@
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>73</v>
@@ -3636,21 +3621,21 @@
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
       <c r="T26" s="9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="49.5">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="27.75">
       <c r="A27" s="6">
         <v>19</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="25"/>
+        <v>118</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="7">
         <v>1</v>
       </c>
@@ -3665,7 +3650,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="M27" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N27" s="9" t="s">
         <v>73</v>
@@ -3678,7 +3663,7 @@
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
       <c r="T27" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="29.25" customHeight="1">
@@ -3686,13 +3671,13 @@
         <v>20</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="25"/>
+        <v>122</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="7">
         <v>1</v>
       </c>
@@ -3707,7 +3692,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N28" s="9" t="s">
         <v>73</v>
@@ -3722,23 +3707,21 @@
       </c>
       <c r="S28" s="6"/>
       <c r="T28" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="27.75">
       <c r="A29" s="6">
         <v>24</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="E29" s="25"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="7">
         <v>1</v>
       </c>
@@ -3771,7 +3754,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="33">
+    <row r="30" spans="1:20" ht="30.75">
       <c r="A30" s="6">
         <v>26</v>
       </c>
@@ -3781,8 +3764,8 @@
       <c r="C30" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="25"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="24"/>
       <c r="F30" s="7">
         <v>1</v>
       </c>
@@ -3813,7 +3796,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="33">
+    <row r="31" spans="1:20" ht="27.75">
       <c r="A31" s="6">
         <v>28</v>
       </c>
@@ -3823,8 +3806,8 @@
       <c r="C31" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="25"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="7">
         <v>1</v>
       </c>
@@ -3855,7 +3838,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="33">
+    <row r="32" spans="1:20" ht="28.5">
       <c r="A32" s="6">
         <v>32</v>
       </c>
@@ -3865,8 +3848,8 @@
       <c r="C32" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="25"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="7">
         <v>1</v>
       </c>
@@ -3899,7 +3882,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="33">
+    <row r="33" spans="1:20" ht="27.75">
       <c r="A33" s="6">
         <v>37</v>
       </c>
@@ -3909,8 +3892,8 @@
       <c r="C33" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="25"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="12">
         <v>2</v>
       </c>
@@ -3937,7 +3920,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="33">
+    <row r="34" spans="1:20" ht="27.75">
       <c r="A34" s="6">
         <v>38</v>
       </c>
@@ -3947,8 +3930,8 @@
       <c r="C34" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="23" t="s">
+      <c r="D34" s="30"/>
+      <c r="E34" s="22" t="s">
         <v>23</v>
       </c>
       <c r="F34" s="12">
@@ -3983,7 +3966,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="33">
+    <row r="35" spans="1:20" ht="30.75">
       <c r="A35" s="6">
         <v>40</v>
       </c>
@@ -3993,8 +3976,8 @@
       <c r="C35" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="25" t="s">
+      <c r="D35" s="30"/>
+      <c r="E35" s="24" t="s">
         <v>150</v>
       </c>
       <c r="F35" s="12">
@@ -4023,7 +4006,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="33">
+    <row r="36" spans="1:20" ht="30.75">
       <c r="A36" s="6">
         <v>41</v>
       </c>
@@ -4033,8 +4016,8 @@
       <c r="C36" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="25"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="12">
         <v>2</v>
       </c>
@@ -4061,7 +4044,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="33">
+    <row r="37" spans="1:20" ht="32.25">
       <c r="A37" s="6">
         <v>42</v>
       </c>
@@ -4071,10 +4054,10 @@
       <c r="C37" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="E37" s="25"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="12">
         <v>2</v>
       </c>
@@ -4105,7 +4088,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" ht="15.75">
       <c r="A38" s="6">
         <v>43</v>
       </c>
@@ -4115,10 +4098,8 @@
       <c r="C38" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="D38" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="E38" s="25"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="12">
         <v>2</v>
       </c>
@@ -4145,7 +4126,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="33">
+    <row r="39" spans="1:20" ht="30.75">
       <c r="A39" s="6">
         <v>45</v>
       </c>
@@ -4155,8 +4136,8 @@
       <c r="C39" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="25" t="s">
+      <c r="D39" s="29"/>
+      <c r="E39" s="24" t="s">
         <v>164</v>
       </c>
       <c r="F39" s="12">
@@ -4185,7 +4166,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="33">
+    <row r="40" spans="1:20" ht="30.75">
       <c r="A40" s="6">
         <v>47</v>
       </c>
@@ -4195,8 +4176,8 @@
       <c r="C40" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="25" t="s">
+      <c r="D40" s="30"/>
+      <c r="E40" s="24" t="s">
         <v>164</v>
       </c>
       <c r="F40" s="12">
@@ -4225,7 +4206,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="33">
+    <row r="41" spans="1:20" ht="41.25">
       <c r="A41" s="6">
         <v>50</v>
       </c>
@@ -4235,8 +4216,8 @@
       <c r="C41" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="25" t="s">
+      <c r="D41" s="29"/>
+      <c r="E41" s="24" t="s">
         <v>171</v>
       </c>
       <c r="F41" s="12">
@@ -4265,7 +4246,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" ht="27.75">
       <c r="A42" s="6">
         <v>51</v>
       </c>
@@ -4275,10 +4256,8 @@
       <c r="C42" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="D42" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="E42" s="25"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="24"/>
       <c r="F42" s="12">
         <v>2</v>
       </c>
@@ -4304,21 +4283,21 @@
       <c r="R42" s="6"/>
       <c r="S42" s="6"/>
       <c r="T42" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="33">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="30.75">
       <c r="A43" s="6">
         <v>52</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="25"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="24"/>
       <c r="F43" s="12">
         <v>2</v>
       </c>
@@ -4344,21 +4323,21 @@
       <c r="R43" s="6"/>
       <c r="S43" s="6"/>
       <c r="T43" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="33">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="30.75">
       <c r="A44" s="6">
         <v>53</v>
       </c>
       <c r="B44" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C44" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="D44" s="30"/>
-      <c r="E44" s="25" t="s">
+      <c r="D44" s="29"/>
+      <c r="E44" s="24" t="s">
         <v>171</v>
       </c>
       <c r="F44" s="12">
@@ -4390,22 +4369,22 @@
       </c>
       <c r="S44" s="6"/>
       <c r="T44" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" ht="33">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="27.75">
       <c r="A45" s="6">
         <v>54</v>
       </c>
       <c r="B45" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="D45" s="30"/>
+      <c r="E45" s="24" t="s">
         <v>184</v>
-      </c>
-      <c r="D45" s="31"/>
-      <c r="E45" s="25" t="s">
-        <v>185</v>
       </c>
       <c r="F45" s="12">
         <v>2</v>
@@ -4430,21 +4409,21 @@
       <c r="R45" s="6"/>
       <c r="S45" s="6"/>
       <c r="T45" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" ht="33">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="30.75">
       <c r="A46" s="6">
         <v>57</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="C46" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="25"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="24"/>
       <c r="F46" s="12">
         <v>2</v>
       </c>
@@ -4470,21 +4449,21 @@
       <c r="R46" s="6"/>
       <c r="S46" s="6"/>
       <c r="T46" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="15.75">
       <c r="A47" s="6">
         <v>58</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="25"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="24"/>
       <c r="F47" s="12">
         <v>2</v>
       </c>
@@ -4514,21 +4493,21 @@
       </c>
       <c r="S47" s="6"/>
       <c r="T47" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="33">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="27.75">
       <c r="A48" s="6">
         <v>61</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C48" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="C48" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="25"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="24"/>
       <c r="F48" s="12">
         <v>2</v>
       </c>
@@ -4556,21 +4535,21 @@
       </c>
       <c r="S48" s="6"/>
       <c r="T48" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" ht="33">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="30.75">
       <c r="A49" s="6">
         <v>62</v>
       </c>
       <c r="B49" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C49" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="C49" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="D49" s="30"/>
-      <c r="E49" s="25"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="24"/>
       <c r="F49" s="12">
         <v>2</v>
       </c>
@@ -4598,21 +4577,21 @@
       </c>
       <c r="S49" s="6"/>
       <c r="T49" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" ht="33">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="30.75">
       <c r="A50" s="6">
         <v>64</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="25"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="24"/>
       <c r="F50" s="12">
         <v>2</v>
       </c>
@@ -4640,23 +4619,21 @@
       </c>
       <c r="S50" s="6"/>
       <c r="T50" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" ht="33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="30.75">
       <c r="A51" s="6">
         <v>65</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C51" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="D51" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="E51" s="25" t="s">
+      <c r="D51" s="26"/>
+      <c r="E51" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F51" s="12">
@@ -4688,21 +4665,21 @@
       </c>
       <c r="S51" s="6"/>
       <c r="T51" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" ht="33">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="30.75">
       <c r="A52" s="6">
         <v>67</v>
       </c>
       <c r="B52" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C52" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="C52" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="D52" s="31"/>
-      <c r="E52" s="25"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="24"/>
       <c r="F52" s="12">
         <v>2</v>
       </c>
@@ -4726,21 +4703,21 @@
       <c r="R52" s="6"/>
       <c r="S52" s="6"/>
       <c r="T52" s="9" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="15.75">
       <c r="A53" s="6">
         <v>70</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C53" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="D53" s="30"/>
-      <c r="E53" s="25"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="24"/>
       <c r="F53" s="12">
         <v>2</v>
       </c>
@@ -4766,21 +4743,21 @@
       <c r="R53" s="6"/>
       <c r="S53" s="6"/>
       <c r="T53" s="9" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" ht="33">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="30.75">
       <c r="A54" s="6">
         <v>71</v>
       </c>
       <c r="B54" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C54" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="C54" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D54" s="30"/>
-      <c r="E54" s="25"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="24"/>
       <c r="F54" s="12">
         <v>2</v>
       </c>
@@ -4806,21 +4783,21 @@
       <c r="R54" s="6"/>
       <c r="S54" s="6"/>
       <c r="T54" s="9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" ht="33">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" ht="30.75">
       <c r="A55" s="6">
         <v>72</v>
       </c>
       <c r="B55" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C55" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="C55" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="D55" s="30"/>
-      <c r="E55" s="23" t="s">
+      <c r="D55" s="29"/>
+      <c r="E55" s="22" t="s">
         <v>23</v>
       </c>
       <c r="F55" s="12">
@@ -4850,21 +4827,21 @@
       <c r="R55" s="6"/>
       <c r="S55" s="6"/>
       <c r="T55" s="9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" ht="33">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" ht="27.75">
       <c r="A56" s="6">
         <v>73</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C56" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="C56" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="D56" s="31"/>
-      <c r="E56" s="25" t="s">
+      <c r="D56" s="30"/>
+      <c r="E56" s="24" t="s">
         <v>171</v>
       </c>
       <c r="F56" s="12">
@@ -4890,21 +4867,21 @@
       <c r="R56" s="6"/>
       <c r="S56" s="6"/>
       <c r="T56" s="9" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" ht="33">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" ht="30.75">
       <c r="A57" s="6">
         <v>74</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="C57" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="D57" s="31"/>
-      <c r="E57" s="25" t="s">
+      <c r="D57" s="30"/>
+      <c r="E57" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F57" s="12">
@@ -4934,22 +4911,22 @@
       </c>
       <c r="S57" s="6"/>
       <c r="T57" s="9" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" ht="33">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="30.75">
       <c r="A58" s="6">
         <v>77</v>
       </c>
       <c r="B58" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C58" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="C58" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="D58" s="31"/>
-      <c r="E58" s="25" t="s">
-        <v>185</v>
+      <c r="D58" s="30"/>
+      <c r="E58" s="24" t="s">
+        <v>184</v>
       </c>
       <c r="F58" s="12">
         <v>2</v>
@@ -4974,21 +4951,21 @@
       <c r="R58" s="6"/>
       <c r="S58" s="6"/>
       <c r="T58" s="9" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" ht="33">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" ht="27.75">
       <c r="A59" s="6">
         <v>78</v>
       </c>
       <c r="B59" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C59" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="C59" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="D59" s="30"/>
-      <c r="E59" s="25" t="s">
+      <c r="D59" s="29"/>
+      <c r="E59" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F59" s="12">
@@ -5014,21 +4991,21 @@
       <c r="R59" s="6"/>
       <c r="S59" s="6"/>
       <c r="T59" s="9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" ht="33">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" ht="27.75">
       <c r="A60" s="6">
         <v>80</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C60" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="C60" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="D60" s="30"/>
-      <c r="E60" s="25"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="24"/>
       <c r="F60" s="10">
         <v>3</v>
       </c>
@@ -5043,7 +5020,7 @@
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
       <c r="M60" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N60" s="9" t="s">
         <v>73</v>
@@ -5056,21 +5033,21 @@
       <c r="R60" s="6"/>
       <c r="S60" s="6"/>
       <c r="T60" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" ht="15.75">
       <c r="A61" s="6">
         <v>83</v>
       </c>
       <c r="B61" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C61" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="C61" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="D61" s="31"/>
-      <c r="E61" s="25"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="24"/>
       <c r="F61" s="10">
         <v>3</v>
       </c>
@@ -5085,7 +5062,7 @@
       <c r="K61" s="10"/>
       <c r="L61" s="10"/>
       <c r="M61" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N61" s="9" t="s">
         <v>73</v>
@@ -5098,21 +5075,21 @@
       <c r="R61" s="6"/>
       <c r="S61" s="6"/>
       <c r="T61" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" ht="33">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" ht="30.75">
       <c r="A62" s="6">
         <v>84</v>
       </c>
       <c r="B62" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="C62" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="D62" s="31"/>
-      <c r="E62" s="25" t="s">
+      <c r="D62" s="30"/>
+      <c r="E62" s="24" t="s">
         <v>171</v>
       </c>
       <c r="F62" s="10">
@@ -5129,7 +5106,7 @@
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
       <c r="M62" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N62" s="9" t="s">
         <v>73</v>
@@ -5144,21 +5121,21 @@
       <c r="R62" s="6"/>
       <c r="S62" s="6"/>
       <c r="T62" s="9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" ht="33">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" ht="27.75">
       <c r="A63" s="6">
         <v>85</v>
       </c>
       <c r="B63" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C63" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="C63" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="D63" s="30"/>
-      <c r="E63" s="25" t="s">
+      <c r="D63" s="29"/>
+      <c r="E63" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F63" s="10">
@@ -5175,7 +5152,7 @@
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
       <c r="M63" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N63" s="9" t="s">
         <v>73</v>
@@ -5192,21 +5169,21 @@
         <v>1</v>
       </c>
       <c r="T63" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" ht="33">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" ht="27.75">
       <c r="A64" s="6">
         <v>86</v>
       </c>
       <c r="B64" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C64" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="C64" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="D64" s="31"/>
-      <c r="E64" s="25" t="s">
+      <c r="D64" s="30"/>
+      <c r="E64" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F64" s="10">
@@ -5225,7 +5202,7 @@
       </c>
       <c r="L64" s="10"/>
       <c r="M64" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N64" s="9" t="s">
         <v>73</v>
@@ -5238,21 +5215,21 @@
       <c r="R64" s="6"/>
       <c r="S64" s="6"/>
       <c r="T64" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" ht="33">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" ht="30.75">
       <c r="A65" s="6">
         <v>87</v>
       </c>
       <c r="B65" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C65" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="C65" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="D65" s="31"/>
-      <c r="E65" s="25"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="24"/>
       <c r="F65" s="10">
         <v>3</v>
       </c>
@@ -5267,7 +5244,7 @@
       <c r="K65" s="10"/>
       <c r="L65" s="10"/>
       <c r="M65" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N65" s="9" t="s">
         <v>73</v>
@@ -5282,22 +5259,22 @@
       <c r="R65" s="6"/>
       <c r="S65" s="6"/>
       <c r="T65" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" ht="15.75">
       <c r="A66" s="6">
         <v>89</v>
       </c>
       <c r="B66" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C66" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="D66" s="35"/>
+      <c r="E66" s="24" t="s">
         <v>254</v>
-      </c>
-      <c r="D66" s="36"/>
-      <c r="E66" s="25" t="s">
-        <v>255</v>
       </c>
       <c r="F66" s="10">
         <v>3</v>
@@ -5313,7 +5290,7 @@
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
       <c r="M66" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N66" s="9" t="s">
         <v>73</v>
@@ -5326,22 +5303,22 @@
       <c r="R66" s="6"/>
       <c r="S66" s="6"/>
       <c r="T66" s="9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" ht="33">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="27.75">
       <c r="A67" s="6">
         <v>91</v>
       </c>
       <c r="B67" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C67" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="C67" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="D67" s="27"/>
-      <c r="E67" s="25" t="s">
-        <v>255</v>
+      <c r="D67" s="26"/>
+      <c r="E67" s="24" t="s">
+        <v>254</v>
       </c>
       <c r="F67" s="10">
         <v>3</v>
@@ -5357,7 +5334,7 @@
       <c r="K67" s="10"/>
       <c r="L67" s="10"/>
       <c r="M67" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N67" s="9" t="s">
         <v>73</v>
@@ -5370,22 +5347,22 @@
       <c r="R67" s="6"/>
       <c r="S67" s="6"/>
       <c r="T67" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" ht="49.5">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" ht="45.75">
       <c r="A68" s="6">
         <v>92</v>
       </c>
       <c r="B68" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C68" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="C68" s="21" t="s">
+      <c r="D68" s="36"/>
+      <c r="E68" s="24" t="s">
         <v>263</v>
-      </c>
-      <c r="D68" s="37"/>
-      <c r="E68" s="25" t="s">
-        <v>264</v>
       </c>
       <c r="F68" s="10">
         <v>3</v>
@@ -5401,7 +5378,7 @@
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
       <c r="M68" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N68" s="9" t="s">
         <v>73</v>
@@ -5416,21 +5393,21 @@
         <v>1</v>
       </c>
       <c r="T68" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" ht="33">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" ht="27.75">
       <c r="A69" s="6">
         <v>93</v>
       </c>
       <c r="B69" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="C69" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="C69" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="D69" s="29"/>
-      <c r="E69" s="25" t="s">
+      <c r="D69" s="28"/>
+      <c r="E69" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F69" s="10">
@@ -5447,7 +5424,7 @@
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
       <c r="M69" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N69" s="9" t="s">
         <v>73</v>
@@ -5462,21 +5439,21 @@
       </c>
       <c r="S69" s="6"/>
       <c r="T69" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" ht="33">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" ht="27.75">
       <c r="A70" s="6">
         <v>94</v>
       </c>
       <c r="B70" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C70" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="C70" s="21" t="s">
-        <v>272</v>
-      </c>
-      <c r="D70" s="31"/>
-      <c r="E70" s="25" t="s">
+      <c r="D70" s="30"/>
+      <c r="E70" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F70" s="10">
@@ -5493,7 +5470,7 @@
       <c r="K70" s="10"/>
       <c r="L70" s="10"/>
       <c r="M70" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N70" s="9" t="s">
         <v>73</v>
@@ -5508,21 +5485,21 @@
       <c r="R70" s="6"/>
       <c r="S70" s="6"/>
       <c r="T70" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="15.75">
       <c r="A71" s="6">
         <v>95</v>
       </c>
       <c r="B71" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C71" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="C71" s="21" t="s">
-        <v>276</v>
-      </c>
-      <c r="D71" s="27"/>
-      <c r="E71" s="25" t="s">
+      <c r="D71" s="26"/>
+      <c r="E71" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F71" s="10">
@@ -5539,7 +5516,7 @@
       <c r="K71" s="10"/>
       <c r="L71" s="10"/>
       <c r="M71" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="N71" s="9" t="s">
         <v>73</v>
@@ -5552,21 +5529,21 @@
       <c r="R71" s="6"/>
       <c r="S71" s="6"/>
       <c r="T71" s="9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="15.75">
       <c r="A72" s="6">
         <v>11</v>
       </c>
       <c r="B72" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C72" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="C72" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="D72" s="30"/>
-      <c r="E72" s="25"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="24"/>
       <c r="F72" s="7">
         <v>1</v>
       </c>
@@ -5581,10 +5558,10 @@
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="N72" s="9" t="s">
         <v>281</v>
-      </c>
-      <c r="N72" s="9" t="s">
-        <v>282</v>
       </c>
       <c r="O72" s="6">
         <v>1</v>
@@ -5594,21 +5571,21 @@
       <c r="R72" s="6"/>
       <c r="S72" s="6"/>
       <c r="T72" s="9" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" ht="33">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="27.75">
       <c r="A73" s="6">
         <v>14</v>
       </c>
       <c r="B73" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C73" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="C73" s="21" t="s">
-        <v>285</v>
-      </c>
-      <c r="D73" s="27"/>
-      <c r="E73" s="25" t="s">
+      <c r="D73" s="26"/>
+      <c r="E73" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F73" s="7">
@@ -5625,10 +5602,10 @@
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
       <c r="M73" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N73" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O73" s="6">
         <v>1</v>
@@ -5640,21 +5617,21 @@
       </c>
       <c r="S73" s="6"/>
       <c r="T73" s="9" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" ht="33">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="30.75">
       <c r="A74" s="6">
         <v>15</v>
       </c>
       <c r="B74" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C74" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="C74" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="D74" s="30"/>
-      <c r="E74" s="25" t="s">
+      <c r="D74" s="29"/>
+      <c r="E74" s="24" t="s">
         <v>171</v>
       </c>
       <c r="F74" s="7">
@@ -5671,10 +5648,10 @@
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="N74" s="9" t="s">
         <v>290</v>
-      </c>
-      <c r="N74" s="9" t="s">
-        <v>291</v>
       </c>
       <c r="O74" s="6"/>
       <c r="P74" s="6"/>
@@ -5682,21 +5659,21 @@
       <c r="R74" s="6"/>
       <c r="S74" s="6"/>
       <c r="T74" s="9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="15.75">
       <c r="A75" s="6">
         <v>23</v>
       </c>
       <c r="B75" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C75" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="C75" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="D75" s="29"/>
-      <c r="E75" s="25"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="24"/>
       <c r="F75" s="7">
         <v>1</v>
       </c>
@@ -5711,10 +5688,10 @@
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N75" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O75" s="6">
         <v>1</v>
@@ -5726,21 +5703,21 @@
       <c r="R75" s="6"/>
       <c r="S75" s="6"/>
       <c r="T75" s="9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" ht="33">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="30.75">
       <c r="A76" s="6">
         <v>29</v>
       </c>
       <c r="B76" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C76" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="C76" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="D76" s="30"/>
-      <c r="E76" s="25"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="24"/>
       <c r="F76" s="7">
         <v>1</v>
       </c>
@@ -5757,10 +5734,10 @@
       </c>
       <c r="L76" s="7"/>
       <c r="M76" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N76" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O76" s="6">
         <v>1</v>
@@ -5772,21 +5749,21 @@
       </c>
       <c r="S76" s="6"/>
       <c r="T76" s="9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" ht="33">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" ht="30.75">
       <c r="A77" s="6">
         <v>30</v>
       </c>
       <c r="B77" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C77" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="C77" s="21" t="s">
-        <v>302</v>
-      </c>
-      <c r="D77" s="30"/>
-      <c r="E77" s="25"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="24"/>
       <c r="F77" s="7">
         <v>1</v>
       </c>
@@ -5801,10 +5778,10 @@
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N77" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O77" s="6">
         <v>1</v>
@@ -5814,21 +5791,21 @@
       <c r="R77" s="6"/>
       <c r="S77" s="6"/>
       <c r="T77" s="9" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" ht="33">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" ht="15.75">
       <c r="A78" s="6">
         <v>31</v>
       </c>
       <c r="B78" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="C78" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="C78" s="21" t="s">
-        <v>306</v>
-      </c>
-      <c r="D78" s="30"/>
-      <c r="E78" s="25"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="24"/>
       <c r="F78" s="7">
         <v>1</v>
       </c>
@@ -5845,10 +5822,10 @@
       </c>
       <c r="L78" s="7"/>
       <c r="M78" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N78" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O78" s="6">
         <v>1</v>
@@ -5858,21 +5835,21 @@
       <c r="R78" s="6"/>
       <c r="S78" s="6"/>
       <c r="T78" s="9" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" ht="33">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" ht="30.75">
       <c r="A79" s="6">
         <v>33</v>
       </c>
       <c r="B79" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C79" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="C79" s="21" t="s">
-        <v>310</v>
-      </c>
-      <c r="D79" s="31"/>
-      <c r="E79" s="25" t="s">
+      <c r="D79" s="30"/>
+      <c r="E79" s="24" t="s">
         <v>171</v>
       </c>
       <c r="F79" s="7">
@@ -5889,10 +5866,10 @@
       <c r="K79" s="7"/>
       <c r="L79" s="7"/>
       <c r="M79" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N79" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O79" s="6">
         <v>1</v>
@@ -5902,22 +5879,22 @@
       <c r="R79" s="6"/>
       <c r="S79" s="6"/>
       <c r="T79" s="9" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" ht="33">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" ht="27.75">
       <c r="A80" s="6">
         <v>36</v>
       </c>
       <c r="B80" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C80" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="C80" s="21" t="s">
-        <v>314</v>
-      </c>
-      <c r="D80" s="31"/>
-      <c r="E80" s="25" t="s">
-        <v>97</v>
+      <c r="D80" s="30"/>
+      <c r="E80" s="24" t="s">
+        <v>98</v>
       </c>
       <c r="F80" s="12">
         <v>2</v>
@@ -5934,7 +5911,7 @@
       <c r="L80" s="12"/>
       <c r="M80" s="14"/>
       <c r="N80" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O80" s="6"/>
       <c r="P80" s="6"/>
@@ -5942,21 +5919,21 @@
       <c r="R80" s="6"/>
       <c r="S80" s="6"/>
       <c r="T80" s="9" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" ht="33">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" ht="30.75">
       <c r="A81" s="6">
         <v>55</v>
       </c>
       <c r="B81" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="C81" s="21" t="s">
         <v>316</v>
       </c>
-      <c r="C81" s="21" t="s">
-        <v>317</v>
-      </c>
-      <c r="D81" s="27"/>
-      <c r="E81" s="23" t="s">
+      <c r="D81" s="26"/>
+      <c r="E81" s="22" t="s">
         <v>23</v>
       </c>
       <c r="F81" s="12">
@@ -5974,7 +5951,7 @@
       <c r="L81" s="12"/>
       <c r="M81" s="14"/>
       <c r="N81" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O81" s="6"/>
       <c r="P81" s="6"/>
@@ -5982,22 +5959,22 @@
       <c r="R81" s="6"/>
       <c r="S81" s="6"/>
       <c r="T81" s="9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" ht="33">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" ht="30.75">
       <c r="A82" s="6">
         <v>56</v>
       </c>
       <c r="B82" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="C82" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="C82" s="21" t="s">
+      <c r="D82" s="29"/>
+      <c r="E82" s="24" t="s">
         <v>320</v>
-      </c>
-      <c r="D82" s="30"/>
-      <c r="E82" s="25" t="s">
-        <v>321</v>
       </c>
       <c r="F82" s="12">
         <v>2</v>
@@ -6014,7 +5991,7 @@
       <c r="L82" s="12"/>
       <c r="M82" s="14"/>
       <c r="N82" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
@@ -6024,21 +6001,21 @@
         <v>1</v>
       </c>
       <c r="T82" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" ht="33">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" ht="27.75">
       <c r="A83" s="6">
         <v>69</v>
       </c>
       <c r="B83" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C83" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="C83" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="D83" s="27"/>
-      <c r="E83" s="23" t="s">
+      <c r="D83" s="26"/>
+      <c r="E83" s="22" t="s">
         <v>23</v>
       </c>
       <c r="F83" s="12">
@@ -6055,10 +6032,10 @@
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N83" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O83" s="6"/>
       <c r="P83" s="6"/>
@@ -6066,21 +6043,21 @@
       <c r="R83" s="6"/>
       <c r="S83" s="6"/>
       <c r="T83" s="9" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" ht="33">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" ht="30.75">
       <c r="A84" s="6">
         <v>76</v>
       </c>
       <c r="B84" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="C84" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="C84" s="21" t="s">
-        <v>328</v>
-      </c>
-      <c r="D84" s="31"/>
-      <c r="E84" s="25"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="24"/>
       <c r="F84" s="12">
         <v>2</v>
       </c>
@@ -6096,7 +6073,7 @@
       <c r="L84" s="12"/>
       <c r="M84" s="14"/>
       <c r="N84" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O84" s="6"/>
       <c r="P84" s="6"/>
@@ -6104,21 +6081,21 @@
       <c r="R84" s="6"/>
       <c r="S84" s="6"/>
       <c r="T84" s="9" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" ht="33">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" ht="30.75">
       <c r="A85" s="6">
         <v>79</v>
       </c>
       <c r="B85" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C85" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="C85" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="D85" s="30"/>
-      <c r="E85" s="25" t="s">
+      <c r="D85" s="29"/>
+      <c r="E85" s="24" t="s">
         <v>171</v>
       </c>
       <c r="F85" s="10">
@@ -6137,10 +6114,10 @@
       </c>
       <c r="L85" s="10"/>
       <c r="M85" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N85" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6"/>
@@ -6150,22 +6127,22 @@
       <c r="R85" s="6"/>
       <c r="S85" s="6"/>
       <c r="T85" s="9" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" ht="33">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" ht="27.75">
       <c r="A86" s="6">
         <v>90</v>
       </c>
       <c r="B86" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="C86" s="21" t="s">
         <v>334</v>
       </c>
-      <c r="C86" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="D86" s="30"/>
-      <c r="E86" s="25" t="s">
-        <v>185</v>
+      <c r="D86" s="29"/>
+      <c r="E86" s="24" t="s">
+        <v>184</v>
       </c>
       <c r="F86" s="10">
         <v>3</v>
@@ -6181,10 +6158,10 @@
       <c r="K86" s="10"/>
       <c r="L86" s="10"/>
       <c r="M86" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N86" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O86" s="6">
         <v>1</v>
@@ -6198,21 +6175,21 @@
         <v>1</v>
       </c>
       <c r="T86" s="9" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="87" spans="1:20" ht="33">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" ht="30.75">
       <c r="A87" s="6">
         <v>8</v>
       </c>
       <c r="B87" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="C87" s="21" t="s">
         <v>338</v>
       </c>
-      <c r="C87" s="21" t="s">
-        <v>339</v>
-      </c>
-      <c r="D87" s="31"/>
-      <c r="E87" s="25"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="24"/>
       <c r="F87" s="7">
         <v>1</v>
       </c>
@@ -6227,10 +6204,10 @@
       <c r="K87" s="7"/>
       <c r="L87" s="7"/>
       <c r="M87" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="N87" s="9" t="s">
         <v>340</v>
-      </c>
-      <c r="N87" s="9" t="s">
-        <v>341</v>
       </c>
       <c r="O87" s="6">
         <v>1</v>
@@ -6240,21 +6217,21 @@
       <c r="R87" s="6"/>
       <c r="S87" s="6"/>
       <c r="T87" s="9" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" ht="33">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" ht="15.75">
       <c r="A88" s="6">
         <v>12</v>
       </c>
       <c r="B88" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C88" s="21" t="s">
         <v>343</v>
       </c>
-      <c r="C88" s="21" t="s">
-        <v>344</v>
-      </c>
-      <c r="D88" s="30"/>
-      <c r="E88" s="25"/>
+      <c r="D88" s="29"/>
+      <c r="E88" s="24"/>
       <c r="F88" s="7">
         <v>1</v>
       </c>
@@ -6269,10 +6246,10 @@
       <c r="K88" s="7"/>
       <c r="L88" s="7"/>
       <c r="M88" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="N88" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O88" s="6"/>
       <c r="P88" s="6"/>
@@ -6282,21 +6259,21 @@
       </c>
       <c r="S88" s="6"/>
       <c r="T88" s="9" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="89" spans="1:20">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" ht="15.75">
       <c r="A89" s="6">
         <v>25</v>
       </c>
       <c r="B89" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="C89" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="C89" s="21" t="s">
-        <v>348</v>
-      </c>
-      <c r="D89" s="31"/>
-      <c r="E89" s="25"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="24"/>
       <c r="F89" s="7">
         <v>1</v>
       </c>
@@ -6311,10 +6288,10 @@
       <c r="K89" s="7"/>
       <c r="L89" s="7"/>
       <c r="M89" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N89" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O89" s="6">
         <v>1</v>
@@ -6324,23 +6301,21 @@
       <c r="R89" s="6"/>
       <c r="S89" s="6"/>
       <c r="T89" s="9" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="90" spans="1:20" ht="33">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" ht="27.75">
       <c r="A90" s="6">
         <v>34</v>
       </c>
       <c r="B90" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C90" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="C90" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="D90" s="30" t="s">
-        <v>353</v>
-      </c>
-      <c r="E90" s="25"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="24"/>
       <c r="F90" s="12">
         <v>2</v>
       </c>
@@ -6356,7 +6331,7 @@
       <c r="L90" s="12"/>
       <c r="M90" s="14"/>
       <c r="N90" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O90" s="6">
         <v>1</v>
@@ -6368,21 +6343,21 @@
       </c>
       <c r="S90" s="6"/>
       <c r="T90" s="9" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="91" spans="1:20">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" ht="15.75">
       <c r="A91" s="6">
         <v>35</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="D91" s="30"/>
-      <c r="E91" s="25"/>
+        <v>354</v>
+      </c>
+      <c r="D91" s="29"/>
+      <c r="E91" s="24"/>
       <c r="F91" s="12">
         <v>2</v>
       </c>
@@ -6398,7 +6373,7 @@
       <c r="L91" s="12"/>
       <c r="M91" s="14"/>
       <c r="N91" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O91" s="6"/>
       <c r="P91" s="6"/>
@@ -6410,21 +6385,21 @@
         <v>1</v>
       </c>
       <c r="T91" s="9" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="92" spans="1:20" ht="33">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" ht="28.5">
       <c r="A92" s="6">
         <v>44</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="D92" s="32"/>
-      <c r="E92" s="25"/>
+        <v>357</v>
+      </c>
+      <c r="D92" s="31"/>
+      <c r="E92" s="24"/>
       <c r="F92" s="12">
         <v>2</v>
       </c>
@@ -6440,7 +6415,7 @@
       <c r="L92" s="12"/>
       <c r="M92" s="14"/>
       <c r="N92" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O92" s="6"/>
       <c r="P92" s="6"/>
@@ -6448,23 +6423,21 @@
       <c r="R92" s="6"/>
       <c r="S92" s="6"/>
       <c r="T92" s="9" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="93" spans="1:20" ht="33">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" ht="30.75">
       <c r="A93" s="6">
         <v>46</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="C93" s="35" t="s">
-        <v>362</v>
-      </c>
-      <c r="D93" s="31" t="s">
-        <v>363</v>
-      </c>
-      <c r="E93" s="25"/>
+        <v>359</v>
+      </c>
+      <c r="C93" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="D93" s="30"/>
+      <c r="E93" s="24"/>
       <c r="F93" s="12">
         <v>2</v>
       </c>
@@ -6480,7 +6453,7 @@
       <c r="L93" s="12"/>
       <c r="M93" s="14"/>
       <c r="N93" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6"/>
@@ -6490,21 +6463,21 @@
       </c>
       <c r="S93" s="6"/>
       <c r="T93" s="9" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="94" spans="1:20" ht="33">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" ht="15.75">
       <c r="A94" s="6">
         <v>48</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>366</v>
-      </c>
-      <c r="D94" s="30"/>
-      <c r="E94" s="25"/>
+        <v>363</v>
+      </c>
+      <c r="D94" s="29"/>
+      <c r="E94" s="24"/>
       <c r="F94" s="12">
         <v>2</v>
       </c>
@@ -6519,10 +6492,10 @@
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
       <c r="M94" s="14" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="N94" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O94" s="6"/>
       <c r="P94" s="6"/>
@@ -6530,21 +6503,21 @@
       <c r="R94" s="6"/>
       <c r="S94" s="6"/>
       <c r="T94" s="9" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="95" spans="1:20" ht="33">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" ht="30.75">
       <c r="A95" s="6">
         <v>49</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>370</v>
-      </c>
-      <c r="D95" s="27"/>
-      <c r="E95" s="38" t="s">
+        <v>367</v>
+      </c>
+      <c r="D95" s="26"/>
+      <c r="E95" s="37" t="s">
         <v>23</v>
       </c>
       <c r="F95" s="12">
@@ -6562,7 +6535,7 @@
       <c r="L95" s="12"/>
       <c r="M95" s="14"/>
       <c r="N95" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O95" s="6">
         <v>1</v>
@@ -6574,7 +6547,7 @@
       </c>
       <c r="S95" s="6"/>
       <c r="T95" s="9" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="96" spans="1:20" ht="20.45" customHeight="1">
@@ -6582,14 +6555,14 @@
         <v>59</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C96" s="21" t="s">
-        <v>373</v>
-      </c>
-      <c r="D96" s="31"/>
-      <c r="E96" s="25" t="s">
-        <v>255</v>
+        <v>370</v>
+      </c>
+      <c r="D96" s="30"/>
+      <c r="E96" s="24" t="s">
+        <v>254</v>
       </c>
       <c r="F96" s="12">
         <v>2</v>
@@ -6606,7 +6579,7 @@
       <c r="L96" s="12"/>
       <c r="M96" s="14"/>
       <c r="N96" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O96" s="6"/>
       <c r="P96" s="6"/>
@@ -6614,21 +6587,21 @@
       <c r="R96" s="6"/>
       <c r="S96" s="6"/>
       <c r="T96" s="9" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="97" spans="1:20" ht="33">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" ht="27.75">
       <c r="A97" s="6">
         <v>66</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>376</v>
-      </c>
-      <c r="D97" s="27"/>
-      <c r="E97" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="D97" s="26"/>
+      <c r="E97" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F97" s="12">
@@ -6646,7 +6619,7 @@
       <c r="L97" s="12"/>
       <c r="M97" s="14"/>
       <c r="N97" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O97" s="6"/>
       <c r="P97" s="6"/>
@@ -6654,21 +6627,21 @@
       <c r="R97" s="6"/>
       <c r="S97" s="6"/>
       <c r="T97" s="9" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="98" spans="1:20" ht="33">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" ht="30.75">
       <c r="A98" s="6">
         <v>75</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>379</v>
-      </c>
-      <c r="D98" s="27"/>
-      <c r="E98" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="D98" s="26"/>
+      <c r="E98" s="24" t="s">
         <v>33</v>
       </c>
       <c r="F98" s="12">
@@ -6686,7 +6659,7 @@
       <c r="L98" s="12"/>
       <c r="M98" s="14"/>
       <c r="N98" s="9" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="O98" s="6"/>
       <c r="P98" s="6"/>
@@ -6694,21 +6667,21 @@
       <c r="R98" s="6"/>
       <c r="S98" s="6"/>
       <c r="T98" s="9" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="99" spans="1:20" ht="33">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" ht="30.75">
       <c r="A99" s="6">
         <v>81</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>383</v>
-      </c>
-      <c r="D99" s="28"/>
-      <c r="E99" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="D99" s="27"/>
+      <c r="E99" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F99" s="10">
@@ -6725,10 +6698,10 @@
       <c r="K99" s="10"/>
       <c r="L99" s="10"/>
       <c r="M99" s="9" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="N99" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O99" s="6">
         <v>1</v>
@@ -6740,18 +6713,18 @@
       <c r="R99" s="6"/>
       <c r="S99" s="6"/>
       <c r="T99" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="100" spans="1:20" ht="33">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" ht="30.75">
       <c r="A100" s="6">
         <v>96</v>
       </c>
-      <c r="B100" s="34" t="s">
-        <v>386</v>
+      <c r="B100" s="33" t="s">
+        <v>383</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D100" s="20"/>
       <c r="E100" s="18"/>
@@ -6769,10 +6742,10 @@
       <c r="K100" s="10"/>
       <c r="L100" s="10"/>
       <c r="M100" s="9" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="N100" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O100" s="6">
         <v>1</v>
@@ -6784,12 +6757,12 @@
       <c r="R100" s="6"/>
       <c r="S100" s="6"/>
       <c r="T100" s="9" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="101" spans="1:20">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" ht="15.75">
       <c r="A101" s="9"/>
-      <c r="B101" s="33"/>
+      <c r="B101" s="32"/>
       <c r="C101" s="9"/>
       <c r="D101" s="19"/>
       <c r="E101" s="9"/>
@@ -6800,7 +6773,7 @@
       <c r="J101" s="6"/>
       <c r="K101" s="6"/>
       <c r="L101" s="6" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="M101" s="9" t="s">
         <v>25</v>
@@ -6816,7 +6789,7 @@
       <c r="S101" s="9"/>
       <c r="T101" s="9"/>
     </row>
-    <row r="102" spans="1:20" ht="30">
+    <row r="102" spans="1:20" ht="30.75">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -6829,10 +6802,10 @@
       <c r="J102" s="6"/>
       <c r="K102" s="6"/>
       <c r="L102" s="6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="M102" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N102" s="9">
         <f>COUNTIF($N$5:$N$100,M102)</f>
@@ -6845,7 +6818,7 @@
       <c r="S102" s="9"/>
       <c r="T102" s="9"/>
     </row>
-    <row r="103" spans="1:20">
+    <row r="103" spans="1:20" ht="15.75">
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
@@ -6858,10 +6831,10 @@
       <c r="J103" s="6"/>
       <c r="K103" s="6"/>
       <c r="L103" s="6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="M103" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N103" s="9">
         <f>COUNTIF($N$5:$N$100,M103)</f>
@@ -6874,7 +6847,7 @@
       <c r="S103" s="9"/>
       <c r="T103" s="9"/>
     </row>
-    <row r="104" spans="1:20">
+    <row r="104" spans="1:20" ht="30.75">
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
@@ -6887,7 +6860,7 @@
       <c r="J104" s="6"/>
       <c r="K104" s="6"/>
       <c r="L104" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="M104" s="9" t="s">
         <v>73</v>
@@ -6950,7 +6923,7 @@
     <mergeCell ref="M3:M4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:E1 A93:B93 D93:XFD93 A94:XFD1048576 A92:C92 E92:XFD92 A5:XFD66 A67:C67 E67:XFD67 A68:XFD91">
+  <conditionalFormatting sqref="A1:E1 A5:XFD66 A67:C67 E67:XFD67 A68:XFD91 A92:C92 E92:XFD92 A93:B93 D93:XFD93 A94:XFD1048576">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"해양 선박 관련 기술"</formula>
     </cfRule>
@@ -7064,9 +7037,11 @@
     <hyperlink ref="C71" r:id="rId92" xr:uid="{09CAE909-5DC9-418E-8455-6BA0ADED58D4}"/>
     <hyperlink ref="C18" r:id="rId93" xr:uid="{4BFF76A0-3264-4CF4-B268-C15BB1CAEFD8}"/>
     <hyperlink ref="C93" r:id="rId94" xr:uid="{BD99E754-824A-44F6-A1C4-89E226012665}"/>
+    <hyperlink ref="C19" r:id="rId95" xr:uid="{18C5DA7B-D275-4DAE-8863-4AC68972ED86}"/>
+    <hyperlink ref="C20" r:id="rId96" xr:uid="{D831EE1B-2413-4ACA-B297-31D966148365}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" r:id="rId95"/>
+  <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" r:id="rId97"/>
 </worksheet>
 </file>
 
@@ -7082,6 +7057,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101003F0E1D52D3165C43B71876C50E262561" ma:contentTypeVersion="12" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="2ad6e6e47ce7ca690a3b0732f8c58809">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1ec7bdc9-c35f-44fb-bc12-eea0df72f52c" xmlns:ns3="0085f31d-9ba7-42e2-9355-3cfee2649550" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d527007f536823eb2a0f11db1a80cd8" ns2:_="" ns3:_="">
     <xsd:import namespace="1ec7bdc9-c35f-44fb-bc12-eea0df72f52c"/>
@@ -7282,23 +7266,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25E48C8B-3F93-42B5-BC1A-441EBCBD88B9}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C85D601E-4F51-4558-A344-0A26E73BC774}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3862B381-0521-4BC3-A226-0E3E2025679D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3862B381-0521-4BC3-A226-0E3E2025679D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B17F2E5-C8C5-4C1A-90BD-A73C793C8DC3}"/>
 </file>
</xml_diff>